<commit_message>
tests for Index class added
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="250">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,6 +1327,15 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
documentation of composition namespace improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="250">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1384,9 @@
       <c r="A17" t="s">
         <v>14</v>
       </c>
+      <c r="B17" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="C17" s="5" t="s">
         <v>248</v>
       </c>
@@ -1395,15 +1398,42 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
+      <c r="B18" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
+      <c r="B19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentation and UT namespaces improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="250">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,6 +1454,9 @@
       <c r="A22" t="s">
         <v>19</v>
       </c>
+      <c r="B22" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="C22" s="5" t="s">
         <v>248</v>
       </c>
@@ -1464,6 +1467,15 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Processes utility moved from IO namespace Diagnostics namespace
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="250">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,11 +1482,29 @@
       <c r="A24" t="s">
         <v>21</v>
       </c>
+      <c r="B24" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
+      <c r="B25" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1563,6 +1581,15 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FileSystem abstraction documentation improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="250">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1142,8 +1142,8 @@
   <dimension ref="A2:K248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,6 +1510,9 @@
       <c r="A26" t="s">
         <v>23</v>
       </c>
+      <c r="B26" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>248</v>
       </c>
@@ -1521,36 +1524,78 @@
       <c r="A27" t="s">
         <v>24</v>
       </c>
+      <c r="C27" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
+      <c r="B28" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
+      <c r="D29" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
+      <c r="C30" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
+      <c r="C31" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
+      <c r="C32" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
+      <c r="C33" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1567,16 +1612,25 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
+      <c r="D35" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
+      <c r="D36" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
+      <c r="D37" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1607,15 +1661,24 @@
       <c r="A40" t="s">
         <v>37</v>
       </c>
+      <c r="D40" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
+      <c r="D41" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
IDirectory.GetFiles() API changed to EnumerateFiles. It now returns an iterator instead of a collection.
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -1143,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,8 +1524,8 @@
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>248</v>
+      <c r="B27" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>248</v>

</xml_diff>

<commit_message>
IFile.ReadAllLines and IFile.WriteAll APIs moved to extension methods to share implementation with different filesystem implementations
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>Not necessary</t>
+  </si>
+  <si>
+    <t>Foundation\Plainion.Core\IO\FileSystemOperations.cs</t>
   </si>
 </sst>
 </file>
@@ -1139,11 +1142,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K248"/>
+  <dimension ref="A2:K249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,13 +1536,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>248</v>
@@ -1547,13 +1547,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>246</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>248</v>
@@ -1561,13 +1561,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>246</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>248</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>246</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>246</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>246</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>246</v>
@@ -1631,7 +1631,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>248</v>
@@ -1639,7 +1645,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>248</v>
@@ -1647,7 +1653,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>248</v>
@@ -1655,13 +1661,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>248</v>
+        <v>34</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>248</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>246</v>
@@ -1683,7 +1683,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>248</v>
@@ -1691,7 +1697,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>248</v>
@@ -1699,7 +1705,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>248</v>
@@ -1707,10 +1713,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>248</v>
@@ -1718,324 +1721,324 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>248</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>248</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>248</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>248</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>248</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>248</v>
-      </c>
+    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>87</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>248</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>91</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>248</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>248</v>
@@ -2046,442 +2049,442 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>99</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>248</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>106</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>248</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>109</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>121</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D125" s="5" t="s">
-        <v>248</v>
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>131</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D135" s="5" t="s">
-        <v>248</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D142" s="5" t="s">
-        <v>248</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>145</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>248</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>158</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D162" s="5" t="s">
-        <v>248</v>
+        <v>157</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="170" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="6"/>
-      <c r="C170" s="6"/>
-      <c r="D170" s="6"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>166</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D171" s="5" t="s">
-        <v>248</v>
-      </c>
+    <row r="171" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C172" s="5" t="s">
         <v>248</v>
@@ -2492,207 +2495,207 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>170</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D175" s="5" t="s">
-        <v>248</v>
+        <v>169</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>173</v>
-      </c>
-      <c r="C178" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D178" s="5" t="s">
-        <v>248</v>
+        <v>172</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>194</v>
-      </c>
-      <c r="C199" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D199" s="5" t="s">
-        <v>248</v>
+        <v>193</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>198</v>
-      </c>
-      <c r="C203" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D203" s="5" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>198</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="205" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="6"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="6"/>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>200</v>
-      </c>
-      <c r="C206" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D206" s="5" t="s">
-        <v>248</v>
-      </c>
+    <row r="206" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="6"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>248</v>
@@ -2703,244 +2706,255 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>202</v>
+        <v>201</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>212</v>
-      </c>
-      <c r="C218" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D218" s="5" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="C219" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D219" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="231" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="6"/>
-      <c r="C231" s="6"/>
-      <c r="D231" s="6"/>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>225</v>
-      </c>
-      <c r="C232" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D232" s="5" t="s">
-        <v>248</v>
-      </c>
+    <row r="232" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="6"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="C233" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>227</v>
-      </c>
-      <c r="C234" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D234" s="5" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>231</v>
-      </c>
-      <c r="C238" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D238" s="5" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D239" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>233</v>
-      </c>
-      <c r="C240" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D240" s="5" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D241" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>236</v>
-      </c>
-      <c r="C243" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D243" s="5" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>236</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="245" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="6"/>
-      <c r="C245" s="6"/>
-      <c r="D245" s="6"/>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>238</v>
-      </c>
+    <row r="246" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="6"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="6"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="248" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="7"/>
-      <c r="C248" s="7"/>
-      <c r="D248" s="7"/>
+    <row r="249" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="7"/>
+      <c r="C249" s="7"/>
+      <c r="D249" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FileSystem abstraction: tests improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1146,7 +1146,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,6 +1530,9 @@
       <c r="B27" s="5" t="s">
         <v>246</v>
       </c>
+      <c r="C27" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>248</v>
       </c>
@@ -1539,6 +1542,9 @@
         <v>250</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>246</v>
       </c>
       <c r="D28" s="5" t="s">

</xml_diff>

<commit_message>
Logging framework reworked to provide more streamlined extension points.
Behavioral changes:
- now always a logging sink has to be added (Console is no longer the default)

Breaking changes
- LoggingFactory implementation interfaces and classes completely changed
- ConsoleLoggerFactoringImpl removed
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1145,8 +1145,8 @@
   <dimension ref="A2:K249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,6 +1765,9 @@
       <c r="A44" t="s">
         <v>40</v>
       </c>
+      <c r="B44" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="C44" s="5" t="s">
         <v>248</v>
       </c>
@@ -1776,60 +1779,132 @@
       <c r="A45" t="s">
         <v>41</v>
       </c>
+      <c r="B45" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
+      <c r="B46" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
+      <c r="B47" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
+      <c r="B48" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
+      <c r="B49" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
+      <c r="B50" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
+      <c r="B51" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
+      <c r="B52" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
+      <c r="B53" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
+      <c r="B54" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
+      <c r="B55" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LoggerBase introduced LoadConfiguration removed from ILoggerFactory (loading configurations is specific to implementations) maximum logging framework extensibility reference implementation added to RI
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1145,8 +1145,8 @@
   <dimension ref="A2:K249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,7 +1853,7 @@
         <v>241</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>243</v>
@@ -1867,7 +1867,7 @@
         <v>241</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>243</v>
@@ -1880,8 +1880,11 @@
       <c r="B52" s="5" t="s">
         <v>241</v>
       </c>
+      <c r="C52" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="D52" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,7 +1895,7 @@
         <v>241</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>243</v>
@@ -1906,7 +1909,7 @@
         <v>241</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>243</v>
@@ -1920,7 +1923,7 @@
         <v>241</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>243</v>
@@ -1934,7 +1937,7 @@
         <v>241</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>243</v>

</xml_diff>

<commit_message>
Docs for Progress and Serialization improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1146,7 +1146,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,6 +1947,9 @@
       <c r="A57" t="s">
         <v>48</v>
       </c>
+      <c r="B57" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="C57" s="5" t="s">
         <v>243</v>
       </c>
@@ -1958,31 +1961,79 @@
       <c r="A58" t="s">
         <v>49</v>
       </c>
+      <c r="B58" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
+      <c r="B59" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>51</v>
       </c>
+      <c r="B60" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>52</v>
       </c>
+      <c r="B61" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
+      <c r="B62" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>54</v>
       </c>
+      <c r="B63" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="C63" s="5" t="s">
         <v>243</v>
       </c>
@@ -1993,6 +2044,15 @@
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentation for Tasks and Text improved
</commit_message>
<xml_diff>
--- a/doc/ReviewProtocol.xlsx
+++ b/doc/ReviewProtocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="251">
   <si>
     <t>Foundation\Plainion.Core</t>
   </si>
@@ -1146,7 +1146,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1856,7 @@
         <v>243</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>243</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
         <v>243</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,6 +2059,9 @@
       <c r="A65" t="s">
         <v>56</v>
       </c>
+      <c r="B65" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="C65" s="5" t="s">
         <v>243</v>
       </c>
@@ -2070,11 +2073,23 @@
       <c r="A66" t="s">
         <v>57</v>
       </c>
+      <c r="B66" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
+      <c r="B67" s="5" t="s">
+        <v>241</v>
+      </c>
       <c r="C67" s="5" t="s">
         <v>243</v>
       </c>
@@ -2085,6 +2100,12 @@
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>